<commit_message>
stores sign up data for student
</commit_message>
<xml_diff>
--- a/final/FinalProject/StudentData.xlsx
+++ b/final/FinalProject/StudentData.xlsx
@@ -14,12 +14,12 @@
   <sheets>
     <sheet name="StudentData" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Student ID</t>
   </si>
@@ -33,29 +33,42 @@
     <t>Password</t>
   </si>
   <si>
-    <t>Elisha Mugenyi</t>
-  </si>
-  <si>
-    <t>elishamugenyi5@gmail.com</t>
-  </si>
-  <si>
-    <t>19@bav12</t>
+    <t>John Doe</t>
+  </si>
+  <si>
+    <t>john-doe@yahoo.com</t>
+  </si>
+  <si>
+    <t>john@123</t>
+  </si>
+  <si>
+    <t>John Babiha</t>
+  </si>
+  <si>
+    <t>jbgoodboy@gmail.com</t>
+  </si>
+  <si>
+    <t>babi@today</t>
+  </si>
+  <si>
+    <t>Melody truth</t>
+  </si>
+  <si>
+    <t>melody@outlook.com</t>
+  </si>
+  <si>
+    <t>mandazi#23</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -78,9 +91,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -361,50 +373,76 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" customWidth="1"/>
-    <col min="3" max="3" width="28.5703125" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" customWidth="1"/>
+    <col min="3" max="3" width="21.85546875" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1">
-      <c r="A1" s="1" t="s">
+    <row r="1">
+      <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="0" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
-      <c r="A2">
-        <v>20231590</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="2">
+      <c r="A2" s="0">
+        <v>20231478</v>
+      </c>
+      <c r="B2" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="0" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0">
+        <v>20231477</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0">
+        <v>20231476</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>